<commit_message>
new wctl template added
</commit_message>
<xml_diff>
--- a/service-loans/template/Template_CW_CMA_TL_WCTL.xlsx
+++ b/service-loans/template/Template_CW_CMA_TL_WCTL.xlsx
@@ -1423,16 +1423,16 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="6" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="164" fontId="3" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="6" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="164" fontId="3" fillId="6" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
@@ -1445,12 +1445,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="6" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -1482,18 +1476,18 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="6" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="6" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="6" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1501,6 +1495,12 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="6" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1813,7 +1813,7 @@
   <dimension ref="A1:XFD86"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="B28" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B67" sqref="B67"/>
       <selection pane="topRight" activeCell="B67" sqref="B67"/>
       <selection pane="bottomLeft" activeCell="B67" sqref="B67"/>
@@ -22271,11 +22271,11 @@
   <dimension ref="A1:Y87"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="7" topLeftCell="B68" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="7" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B67" sqref="B67"/>
       <selection pane="topRight" activeCell="B67" sqref="B67"/>
       <selection pane="bottomLeft" activeCell="B67" sqref="B67"/>
-      <selection pane="bottomRight" activeCell="E87" sqref="E87"/>
+      <selection pane="bottomRight" activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -22286,13 +22286,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="121" t="s">
+      <c r="A1" s="119" t="s">
         <v>75</v>
       </c>
-      <c r="B1" s="121"/>
-      <c r="C1" s="121"/>
-      <c r="D1" s="121"/>
-      <c r="E1" s="121"/>
+      <c r="B1" s="119"/>
+      <c r="C1" s="119"/>
+      <c r="D1" s="119"/>
+      <c r="E1" s="119"/>
       <c r="F1" s="35"/>
       <c r="G1" s="36"/>
       <c r="H1" s="36"/>
@@ -22313,13 +22313,13 @@
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A2" s="122" t="s">
+      <c r="A2" s="120" t="s">
         <v>74</v>
       </c>
-      <c r="B2" s="122"/>
-      <c r="C2" s="122"/>
-      <c r="D2" s="122"/>
-      <c r="E2" s="122"/>
+      <c r="B2" s="120"/>
+      <c r="C2" s="120"/>
+      <c r="D2" s="120"/>
+      <c r="E2" s="120"/>
       <c r="F2" s="39"/>
       <c r="G2" s="39"/>
       <c r="H2" s="39"/>
@@ -22330,13 +22330,13 @@
       <c r="M2" s="39"/>
     </row>
     <row r="3" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="125" t="s">
+      <c r="A3" s="123" t="s">
         <v>73</v>
       </c>
-      <c r="B3" s="125"/>
-      <c r="C3" s="125"/>
-      <c r="D3" s="125"/>
-      <c r="E3" s="125"/>
+      <c r="B3" s="123"/>
+      <c r="C3" s="123"/>
+      <c r="D3" s="123"/>
+      <c r="E3" s="123"/>
       <c r="F3" s="41"/>
       <c r="G3" s="41"/>
       <c r="H3" s="41"/>
@@ -22347,11 +22347,11 @@
       <c r="M3" s="41"/>
     </row>
     <row r="4" spans="1:25" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="123" t="s">
+      <c r="A4" s="121" t="s">
         <v>42</v>
       </c>
-      <c r="B4" s="124"/>
-      <c r="C4" s="124"/>
+      <c r="B4" s="122"/>
+      <c r="C4" s="122"/>
       <c r="D4" s="100" t="s">
         <v>41</v>
       </c>
@@ -22482,129 +22482,129 @@
     </row>
     <row r="6" spans="1:25" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="118"/>
-      <c r="B6" s="126" t="str">
+      <c r="B6" s="124" t="str">
         <f>+'Operating Stmt.'!B6:B6</f>
         <v>Audited</v>
       </c>
-      <c r="C6" s="119" t="str">
+      <c r="C6" s="113" t="str">
         <f>+'Operating Stmt.'!C6:C6</f>
         <v>Audited</v>
       </c>
-      <c r="D6" s="119" t="str">
+      <c r="D6" s="113" t="str">
         <f>+'Operating Stmt.'!D6:D6</f>
         <v>Audited</v>
       </c>
-      <c r="E6" s="119" t="str">
+      <c r="E6" s="113" t="str">
         <f>+'Operating Stmt.'!E6:E6</f>
         <v>Estimated</v>
       </c>
-      <c r="F6" s="119" t="str">
+      <c r="F6" s="113" t="str">
         <f>+'Operating Stmt.'!F6:F6</f>
         <v>Projected</v>
       </c>
-      <c r="G6" s="119" t="str">
+      <c r="G6" s="113" t="str">
         <f>+'Operating Stmt.'!G6:G6</f>
         <v>Projected</v>
       </c>
-      <c r="H6" s="119" t="str">
+      <c r="H6" s="113" t="str">
         <f>+'Operating Stmt.'!H6:H6</f>
         <v>Projected</v>
       </c>
-      <c r="I6" s="119" t="str">
+      <c r="I6" s="113" t="str">
         <f>+'Operating Stmt.'!I6:I6</f>
         <v>Projected</v>
       </c>
-      <c r="J6" s="119" t="str">
+      <c r="J6" s="113" t="str">
         <f>+'Operating Stmt.'!J6:J6</f>
         <v>Projected</v>
       </c>
-      <c r="K6" s="119" t="str">
+      <c r="K6" s="113" t="str">
         <f>+'Operating Stmt.'!K6:K6</f>
         <v>Projected</v>
       </c>
-      <c r="L6" s="119" t="str">
+      <c r="L6" s="113" t="str">
         <f>+'Operating Stmt.'!L6:L6</f>
         <v>Projected</v>
       </c>
-      <c r="M6" s="129" t="str">
+      <c r="M6" s="111" t="str">
         <f>+'Operating Stmt.'!M6:M6</f>
         <v>Projected</v>
       </c>
-      <c r="N6" s="111" t="str">
+      <c r="N6" s="127" t="str">
         <f>+'Operating Stmt.'!N6:N6</f>
         <v>Projected</v>
       </c>
-      <c r="O6" s="111" t="str">
+      <c r="O6" s="127" t="str">
         <f>+'Operating Stmt.'!O6:O6</f>
         <v>Projected</v>
       </c>
-      <c r="P6" s="111" t="str">
+      <c r="P6" s="127" t="str">
         <f>+'Operating Stmt.'!P6:P6</f>
         <v>Projected</v>
       </c>
-      <c r="Q6" s="111" t="str">
+      <c r="Q6" s="127" t="str">
         <f>+'Operating Stmt.'!Q6:Q6</f>
         <v>Projected</v>
       </c>
-      <c r="R6" s="111" t="str">
+      <c r="R6" s="127" t="str">
         <f>+'Operating Stmt.'!R6:R6</f>
         <v>Projected</v>
       </c>
-      <c r="S6" s="111" t="str">
+      <c r="S6" s="127" t="str">
         <f>+'Operating Stmt.'!S6:S6</f>
         <v>Projected</v>
       </c>
-      <c r="T6" s="111" t="str">
+      <c r="T6" s="127" t="str">
         <f>+'Operating Stmt.'!T6:T6</f>
         <v>Projected</v>
       </c>
-      <c r="U6" s="111" t="str">
+      <c r="U6" s="127" t="str">
         <f>+'Operating Stmt.'!U6:U6</f>
         <v>Projected</v>
       </c>
-      <c r="V6" s="111" t="str">
+      <c r="V6" s="127" t="str">
         <f>+'Operating Stmt.'!V6:V6</f>
         <v>Projected</v>
       </c>
-      <c r="W6" s="111" t="str">
+      <c r="W6" s="127" t="str">
         <f>+'Operating Stmt.'!W6:W6</f>
         <v>Projected</v>
       </c>
-      <c r="X6" s="111" t="str">
+      <c r="X6" s="127" t="str">
         <f>+'Operating Stmt.'!X6:X6</f>
         <v>Projected</v>
       </c>
-      <c r="Y6" s="113" t="str">
+      <c r="Y6" s="129" t="str">
         <f>+'Operating Stmt.'!Y6:Y6</f>
         <v>Projected</v>
       </c>
     </row>
     <row r="7" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="118"/>
-      <c r="B7" s="127"/>
-      <c r="C7" s="128"/>
-      <c r="D7" s="128"/>
-      <c r="E7" s="128"/>
-      <c r="F7" s="120"/>
-      <c r="G7" s="120"/>
-      <c r="H7" s="120"/>
-      <c r="I7" s="120"/>
-      <c r="J7" s="120"/>
-      <c r="K7" s="120"/>
-      <c r="L7" s="120"/>
-      <c r="M7" s="130"/>
-      <c r="N7" s="112"/>
-      <c r="O7" s="112"/>
-      <c r="P7" s="112"/>
-      <c r="Q7" s="112"/>
-      <c r="R7" s="112"/>
-      <c r="S7" s="112"/>
-      <c r="T7" s="112"/>
-      <c r="U7" s="112"/>
-      <c r="V7" s="112"/>
-      <c r="W7" s="112"/>
-      <c r="X7" s="112"/>
-      <c r="Y7" s="114"/>
+      <c r="B7" s="125"/>
+      <c r="C7" s="126"/>
+      <c r="D7" s="126"/>
+      <c r="E7" s="126"/>
+      <c r="F7" s="114"/>
+      <c r="G7" s="114"/>
+      <c r="H7" s="114"/>
+      <c r="I7" s="114"/>
+      <c r="J7" s="114"/>
+      <c r="K7" s="114"/>
+      <c r="L7" s="114"/>
+      <c r="M7" s="112"/>
+      <c r="N7" s="128"/>
+      <c r="O7" s="128"/>
+      <c r="P7" s="128"/>
+      <c r="Q7" s="128"/>
+      <c r="R7" s="128"/>
+      <c r="S7" s="128"/>
+      <c r="T7" s="128"/>
+      <c r="U7" s="128"/>
+      <c r="V7" s="128"/>
+      <c r="W7" s="128"/>
+      <c r="X7" s="128"/>
+      <c r="Y7" s="130"/>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" s="44" t="s">
@@ -25513,12 +25513,18 @@
   </sheetData>
   <sheetProtection password="CF53" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="30">
-    <mergeCell ref="M6:M7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="K6:K7"/>
-    <mergeCell ref="J6:J7"/>
-    <mergeCell ref="I6:I7"/>
+    <mergeCell ref="X6:X7"/>
+    <mergeCell ref="Y6:Y7"/>
+    <mergeCell ref="S6:S7"/>
+    <mergeCell ref="T6:T7"/>
+    <mergeCell ref="U6:U7"/>
+    <mergeCell ref="V6:V7"/>
+    <mergeCell ref="W6:W7"/>
+    <mergeCell ref="N6:N7"/>
+    <mergeCell ref="O6:O7"/>
+    <mergeCell ref="P6:P7"/>
+    <mergeCell ref="Q6:Q7"/>
+    <mergeCell ref="R6:R7"/>
     <mergeCell ref="A33:A34"/>
     <mergeCell ref="A5:A7"/>
     <mergeCell ref="L6:L7"/>
@@ -25531,18 +25537,12 @@
     <mergeCell ref="C6:C7"/>
     <mergeCell ref="D6:D7"/>
     <mergeCell ref="E6:E7"/>
-    <mergeCell ref="N6:N7"/>
-    <mergeCell ref="O6:O7"/>
-    <mergeCell ref="P6:P7"/>
-    <mergeCell ref="Q6:Q7"/>
-    <mergeCell ref="R6:R7"/>
-    <mergeCell ref="X6:X7"/>
-    <mergeCell ref="Y6:Y7"/>
-    <mergeCell ref="S6:S7"/>
-    <mergeCell ref="T6:T7"/>
-    <mergeCell ref="U6:U7"/>
-    <mergeCell ref="V6:V7"/>
-    <mergeCell ref="W6:W7"/>
+    <mergeCell ref="M6:M7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="K6:K7"/>
+    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="I6:I7"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11:M13 B17:M32 B82:M83 B41:M53 B67:M80 B57:Y57 N45:Y45">
@@ -25579,13 +25579,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="121" t="s">
+      <c r="A1" s="119" t="s">
         <v>97</v>
       </c>
-      <c r="B1" s="121"/>
-      <c r="C1" s="121"/>
-      <c r="D1" s="121"/>
-      <c r="E1" s="121"/>
+      <c r="B1" s="119"/>
+      <c r="C1" s="119"/>
+      <c r="D1" s="119"/>
+      <c r="E1" s="119"/>
       <c r="F1" s="36"/>
       <c r="G1" s="36"/>
       <c r="H1" s="36"/>
@@ -25606,13 +25606,13 @@
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A2" s="122" t="s">
+      <c r="A2" s="120" t="s">
         <v>74</v>
       </c>
-      <c r="B2" s="122"/>
-      <c r="C2" s="122"/>
-      <c r="D2" s="122"/>
-      <c r="E2" s="122"/>
+      <c r="B2" s="120"/>
+      <c r="C2" s="120"/>
+      <c r="D2" s="120"/>
+      <c r="E2" s="120"/>
       <c r="F2" s="39"/>
       <c r="G2" s="39"/>
       <c r="H2" s="39"/>
@@ -25623,13 +25623,13 @@
       <c r="M2" s="39"/>
     </row>
     <row r="3" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="125" t="s">
+      <c r="A3" s="123" t="s">
         <v>73</v>
       </c>
-      <c r="B3" s="125"/>
-      <c r="C3" s="125"/>
-      <c r="D3" s="125"/>
-      <c r="E3" s="125"/>
+      <c r="B3" s="123"/>
+      <c r="C3" s="123"/>
+      <c r="D3" s="123"/>
+      <c r="E3" s="123"/>
       <c r="F3" s="41"/>
       <c r="G3" s="41"/>
       <c r="H3" s="41"/>
@@ -25640,11 +25640,11 @@
       <c r="M3" s="41"/>
     </row>
     <row r="4" spans="1:25" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="123" t="s">
+      <c r="A4" s="121" t="s">
         <v>42</v>
       </c>
-      <c r="B4" s="124"/>
-      <c r="C4" s="124"/>
+      <c r="B4" s="122"/>
+      <c r="C4" s="122"/>
       <c r="D4" s="101" t="s">
         <v>41</v>
       </c>
@@ -25673,7 +25673,7 @@
       <c r="Y4" s="42"/>
     </row>
     <row r="5" spans="1:25" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="134" t="s">
+      <c r="A5" s="132" t="s">
         <v>96</v>
       </c>
       <c r="B5" s="84">
@@ -25774,117 +25774,117 @@
       </c>
     </row>
     <row r="6" spans="1:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="135"/>
-      <c r="B6" s="126" t="str">
+      <c r="A6" s="133"/>
+      <c r="B6" s="124" t="str">
         <f>Liabilities!B6</f>
         <v>Audited</v>
       </c>
-      <c r="C6" s="119" t="str">
+      <c r="C6" s="113" t="str">
         <f>Liabilities!C6</f>
         <v>Audited</v>
       </c>
-      <c r="D6" s="119" t="str">
+      <c r="D6" s="113" t="str">
         <f>Liabilities!D6</f>
         <v>Audited</v>
       </c>
-      <c r="E6" s="119" t="str">
+      <c r="E6" s="113" t="str">
         <f>Liabilities!E6</f>
         <v>Estimated</v>
       </c>
-      <c r="F6" s="119" t="str">
+      <c r="F6" s="113" t="str">
         <f>Liabilities!F6</f>
         <v>Projected</v>
       </c>
-      <c r="G6" s="119" t="str">
+      <c r="G6" s="113" t="str">
         <f>Liabilities!G6</f>
         <v>Projected</v>
       </c>
-      <c r="H6" s="119" t="str">
+      <c r="H6" s="113" t="str">
         <f>Liabilities!H6</f>
         <v>Projected</v>
       </c>
-      <c r="I6" s="119" t="str">
+      <c r="I6" s="113" t="str">
         <f>Liabilities!I6</f>
         <v>Projected</v>
       </c>
-      <c r="J6" s="119" t="str">
+      <c r="J6" s="113" t="str">
         <f>Liabilities!J6</f>
         <v>Projected</v>
       </c>
-      <c r="K6" s="119" t="str">
+      <c r="K6" s="113" t="str">
         <f>Liabilities!K6</f>
         <v>Projected</v>
       </c>
-      <c r="L6" s="119" t="str">
+      <c r="L6" s="113" t="str">
         <f>Liabilities!L6</f>
         <v>Projected</v>
       </c>
-      <c r="M6" s="129" t="str">
+      <c r="M6" s="111" t="str">
         <f>Liabilities!M6</f>
         <v>Projected</v>
       </c>
-      <c r="N6" s="129" t="str">
+      <c r="N6" s="111" t="str">
         <f>Liabilities!N6</f>
         <v>Projected</v>
       </c>
-      <c r="O6" s="129" t="str">
+      <c r="O6" s="111" t="str">
         <f>Liabilities!O6</f>
         <v>Projected</v>
       </c>
-      <c r="P6" s="129" t="str">
+      <c r="P6" s="111" t="str">
         <f>Liabilities!P6</f>
         <v>Projected</v>
       </c>
-      <c r="Q6" s="129" t="str">
+      <c r="Q6" s="111" t="str">
         <f>Liabilities!Q6</f>
         <v>Projected</v>
       </c>
-      <c r="R6" s="129" t="str">
+      <c r="R6" s="111" t="str">
         <f>Liabilities!R6</f>
         <v>Projected</v>
       </c>
-      <c r="S6" s="129" t="str">
+      <c r="S6" s="111" t="str">
         <f>Liabilities!S6</f>
         <v>Projected</v>
       </c>
-      <c r="T6" s="129" t="str">
+      <c r="T6" s="111" t="str">
         <f>Liabilities!T6</f>
         <v>Projected</v>
       </c>
-      <c r="U6" s="129" t="str">
+      <c r="U6" s="111" t="str">
         <f>Liabilities!U6</f>
         <v>Projected</v>
       </c>
-      <c r="V6" s="129" t="str">
+      <c r="V6" s="111" t="str">
         <f>Liabilities!V6</f>
         <v>Projected</v>
       </c>
-      <c r="W6" s="129" t="str">
+      <c r="W6" s="111" t="str">
         <f>Liabilities!W6</f>
         <v>Projected</v>
       </c>
-      <c r="X6" s="129" t="str">
+      <c r="X6" s="111" t="str">
         <f>Liabilities!X6</f>
         <v>Projected</v>
       </c>
-      <c r="Y6" s="132" t="str">
+      <c r="Y6" s="134" t="str">
         <f>Liabilities!Y6</f>
         <v>Projected</v>
       </c>
     </row>
     <row r="7" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="135"/>
-      <c r="B7" s="127"/>
-      <c r="C7" s="128"/>
-      <c r="D7" s="128"/>
-      <c r="E7" s="128"/>
-      <c r="F7" s="128"/>
-      <c r="G7" s="128"/>
-      <c r="H7" s="128"/>
-      <c r="I7" s="128"/>
-      <c r="J7" s="128"/>
-      <c r="K7" s="128"/>
-      <c r="L7" s="128"/>
+      <c r="A7" s="133"/>
+      <c r="B7" s="125"/>
+      <c r="C7" s="126"/>
+      <c r="D7" s="126"/>
+      <c r="E7" s="126"/>
+      <c r="F7" s="126"/>
+      <c r="G7" s="126"/>
+      <c r="H7" s="126"/>
+      <c r="I7" s="126"/>
+      <c r="J7" s="126"/>
+      <c r="K7" s="126"/>
+      <c r="L7" s="126"/>
       <c r="M7" s="131"/>
       <c r="N7" s="131"/>
       <c r="O7" s="131"/>
@@ -25897,7 +25897,7 @@
       <c r="V7" s="131"/>
       <c r="W7" s="131"/>
       <c r="X7" s="131"/>
-      <c r="Y7" s="133"/>
+      <c r="Y7" s="135"/>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" s="64" t="s">
@@ -26723,27 +26723,27 @@
       <c r="B29" s="68"/>
       <c r="C29" s="68"/>
       <c r="D29" s="68"/>
-      <c r="E29" s="68"/>
-      <c r="F29" s="68"/>
-      <c r="G29" s="68"/>
-      <c r="H29" s="68"/>
-      <c r="I29" s="68"/>
-      <c r="J29" s="68"/>
-      <c r="K29" s="68"/>
-      <c r="L29" s="68"/>
-      <c r="M29" s="47"/>
-      <c r="N29" s="47"/>
-      <c r="O29" s="47"/>
-      <c r="P29" s="47"/>
-      <c r="Q29" s="47"/>
-      <c r="R29" s="47"/>
-      <c r="S29" s="47"/>
-      <c r="T29" s="47"/>
-      <c r="U29" s="47"/>
-      <c r="V29" s="47"/>
-      <c r="W29" s="47"/>
-      <c r="X29" s="47"/>
-      <c r="Y29" s="47"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="4"/>
+      <c r="J29" s="4"/>
+      <c r="K29" s="4"/>
+      <c r="L29" s="4"/>
+      <c r="M29" s="2"/>
+      <c r="N29" s="2"/>
+      <c r="O29" s="2"/>
+      <c r="P29" s="2"/>
+      <c r="Q29" s="2"/>
+      <c r="R29" s="2"/>
+      <c r="S29" s="2"/>
+      <c r="T29" s="2"/>
+      <c r="U29" s="2"/>
+      <c r="V29" s="2"/>
+      <c r="W29" s="2"/>
+      <c r="X29" s="2"/>
+      <c r="Y29" s="2"/>
     </row>
     <row r="30" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A30" s="65"/>
@@ -26779,27 +26779,27 @@
       <c r="B31" s="68"/>
       <c r="C31" s="68"/>
       <c r="D31" s="68"/>
-      <c r="E31" s="68"/>
-      <c r="F31" s="68"/>
-      <c r="G31" s="68"/>
-      <c r="H31" s="68"/>
-      <c r="I31" s="68"/>
-      <c r="J31" s="68"/>
-      <c r="K31" s="68"/>
-      <c r="L31" s="68"/>
-      <c r="M31" s="47"/>
-      <c r="N31" s="47"/>
-      <c r="O31" s="47"/>
-      <c r="P31" s="47"/>
-      <c r="Q31" s="47"/>
-      <c r="R31" s="47"/>
-      <c r="S31" s="47"/>
-      <c r="T31" s="47"/>
-      <c r="U31" s="47"/>
-      <c r="V31" s="47"/>
-      <c r="W31" s="47"/>
-      <c r="X31" s="47"/>
-      <c r="Y31" s="47"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
+      <c r="H31" s="4"/>
+      <c r="I31" s="4"/>
+      <c r="J31" s="4"/>
+      <c r="K31" s="4"/>
+      <c r="L31" s="4"/>
+      <c r="M31" s="2"/>
+      <c r="N31" s="2"/>
+      <c r="O31" s="2"/>
+      <c r="P31" s="2"/>
+      <c r="Q31" s="2"/>
+      <c r="R31" s="2"/>
+      <c r="S31" s="2"/>
+      <c r="T31" s="2"/>
+      <c r="U31" s="2"/>
+      <c r="V31" s="2"/>
+      <c r="W31" s="2"/>
+      <c r="X31" s="2"/>
+      <c r="Y31" s="2"/>
     </row>
     <row r="32" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A32" s="65"/>
@@ -29740,6 +29740,19 @@
   </sheetData>
   <sheetProtection password="CF53" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="29">
+    <mergeCell ref="R6:R7"/>
+    <mergeCell ref="X6:X7"/>
+    <mergeCell ref="Y6:Y7"/>
+    <mergeCell ref="S6:S7"/>
+    <mergeCell ref="T6:T7"/>
+    <mergeCell ref="U6:U7"/>
+    <mergeCell ref="V6:V7"/>
+    <mergeCell ref="W6:W7"/>
+    <mergeCell ref="L6:L7"/>
+    <mergeCell ref="N6:N7"/>
+    <mergeCell ref="O6:O7"/>
+    <mergeCell ref="P6:P7"/>
+    <mergeCell ref="Q6:Q7"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="A3:E3"/>
@@ -29756,19 +29769,6 @@
     <mergeCell ref="I6:I7"/>
     <mergeCell ref="J6:J7"/>
     <mergeCell ref="K6:K7"/>
-    <mergeCell ref="L6:L7"/>
-    <mergeCell ref="N6:N7"/>
-    <mergeCell ref="O6:O7"/>
-    <mergeCell ref="P6:P7"/>
-    <mergeCell ref="Q6:Q7"/>
-    <mergeCell ref="R6:R7"/>
-    <mergeCell ref="X6:X7"/>
-    <mergeCell ref="Y6:Y7"/>
-    <mergeCell ref="S6:S7"/>
-    <mergeCell ref="T6:T7"/>
-    <mergeCell ref="U6:U7"/>
-    <mergeCell ref="V6:V7"/>
-    <mergeCell ref="W6:W7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="50" orientation="portrait" r:id="rId1"/>

</xml_diff>